<commit_message>
0520 crud, element, sql update
</commit_message>
<xml_diff>
--- a/0513_CRUD_MATRIX.xlsx
+++ b/0513_CRUD_MATRIX.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Naver MYBOX\21-s\데베설\git_corp\My-Cinema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\새 폴더\Naver MYBOX\21-s\데베설\git_corp\My-Cinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE95F816-9038-4865-B78A-85A6471052BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEDC9953-0B47-43BF-B819-04E6427AF093}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6120" yWindow="8790" windowWidth="21210" windowHeight="15435" xr2:uid="{BF35880F-C2E3-41AF-9943-8008D55ED834}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BF35880F-C2E3-41AF-9943-8008D55ED834}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>영화를 등록한다</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,6 +64,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>티켓정보를 취소한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화관, 상영관, 좌석을 선택한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>포인트로 할인을 받는다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -72,6 +80,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>결제 후 포인트를 적립한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제 가능시간이 지나면 예매정보를 취소한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화의 예매율 정보를 갱신한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>지역</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -84,6 +104,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>티켓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>결제정보</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -137,58 +161,6 @@
   </si>
   <si>
     <t>U</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예매를 취소한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>U</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>포인트를 적립한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제자가 시청 가능한 영화인지 확인한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화관, 상영관, 좌석을 선택한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제 만료 시간인지 계산한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제완료된 예매정보를 확인한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제완료된 예매정보를 취소한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고객이 키워드를 가지고 영화를 검색한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화관을 선택해 상영중인 영화를 검색한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상영중인 영화를 예매율 순으로 정렬한다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -553,277 +525,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FCE492-328D-4B73-9660-E6C5C9C9FD95}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="44.25" customWidth="1"/>
+    <col min="1" max="1" width="44.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
       <c r="M1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="L7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="L8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" t="s">
-        <v>24</v>
-      </c>
-      <c r="N16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="I18" t="s">
-        <v>24</v>
-      </c>
-      <c r="L18" t="s">
-        <v>24</v>
-      </c>
-      <c r="N18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="I20" t="s">
-        <v>28</v>
-      </c>
-      <c r="L20" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>